<commit_message>
Added environment configuration file scouting2019.yml
</commit_message>
<xml_diff>
--- a/server/web/data/turing_2018_2018Apr20_090254.xlsx
+++ b/server/web/data/turing_2018_2018Apr20_090254.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stacy\OneDrive\Projects\scouting\scouting2017\irsScouting2017\server\web\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F28558E-6B99-4B59-B96A-5BC5167AA63A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{0F28558E-6B99-4B59-B96A-5BC5167AA63A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{7C824DE9-DA23-4966-88AF-F16621132633}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -502,13 +502,21 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="6" max="7" width="9.06640625" style="6"/>
-    <col min="10" max="11" width="9.06640625" style="6"/>
+    <col min="4" max="4" width="11.46484375" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" customWidth="1"/>
+    <col min="6" max="6" width="11.19921875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.3984375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" customWidth="1"/>
+    <col min="9" max="9" width="10.53125" customWidth="1"/>
+    <col min="10" max="10" width="12.86328125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="13.265625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="12.265625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
@@ -5123,7 +5131,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A6:X73" xr:uid="{AD65B7FA-99D8-404F-A1F2-5BFFF7F777E8}">
-    <sortState ref="A7:X73">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:X73">
       <sortCondition descending="1" ref="E6:E73"/>
     </sortState>
   </autoFilter>

</xml_diff>